<commit_message>
Add 'avenant evision loyer EA' functionality
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2024.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2024.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,7 +429,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>044/FES VILLE /AV4</v>
+        <v>044/FES VILLE /AV6</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
@@ -449,61 +449,61 @@
       <c r="G2">
         <v>15</v>
       </c>
-      <c r="H2">
-        <v>10001</v>
+      <c r="H2" t="str">
+        <v>--</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>1500.15</v>
+      <c r="J2" t="str">
+        <v>--</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>10000</v>
+        <v>600</v>
+      </c>
+      <c r="N2" t="str">
+        <v>--</v>
       </c>
       <c r="O2">
-        <v>8500.85</v>
+        <v>9400</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>044/FES VILLE /AV6</v>
       </c>
       <c r="B3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>K5443645</v>
       </c>
       <c r="D3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>KHADIJA LALA</v>
       </c>
       <c r="E3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>non</v>
       </c>
       <c r="F3" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>mensuelle</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
       </c>
       <c r="H3">
-        <v>10001</v>
+        <v>30000</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>1500.15</v>
+        <v>4500</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -518,12 +518,106 @@
         <v>10000</v>
       </c>
       <c r="O3">
-        <v>8500.85</v>
+        <v>25500</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>044/FES VILLE /AV6</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C4" t="str">
+        <v>K5443645</v>
+      </c>
+      <c r="D4" t="str">
+        <v>KHADIJA LALA</v>
+      </c>
+      <c r="E4" t="str">
+        <v>non</v>
+      </c>
+      <c r="F4" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4" t="str">
+        <v>--</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <v>--</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>5000</v>
+      </c>
+      <c r="M4">
+        <v>700</v>
+      </c>
+      <c r="N4" t="str">
+        <v>--</v>
+      </c>
+      <c r="O4">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="B5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H5">
+        <v>30000</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>4500</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>15000</v>
+      </c>
+      <c r="M5">
+        <v>1300</v>
+      </c>
+      <c r="N5">
+        <v>10000</v>
+      </c>
+      <c r="O5">
+        <v>39200</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix rappel AV auto with manual
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2024.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2024.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,16 +429,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>555/RRR/AV3</v>
+        <v>444/444</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>B171710</v>
+        <v>IR801997</v>
       </c>
       <c r="D2" t="str">
-        <v>NADIA BADRANE</v>
+        <v>NOUBAIL MOHAMMED</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -462,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>16000</v>
+        <v>22500</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -471,21 +471,21 @@
         <v>--</v>
       </c>
       <c r="O2">
-        <v>16000</v>
+        <v>22500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>555/RRR/AV3</v>
+        <v>444/444</v>
       </c>
       <c r="B3" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>IB43905</v>
+        <v>B219321</v>
       </c>
       <c r="D3" t="str">
-        <v>NHILA BELGACEM</v>
+        <v>JEMAA HORMI</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -509,7 +509,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>16000</v>
+        <v>22500</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -518,21 +518,21 @@
         <v>--</v>
       </c>
       <c r="O3">
-        <v>16000</v>
+        <v>22500</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>555/RRR/AV3</v>
+        <v>444/444</v>
       </c>
       <c r="B4" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C4" t="str">
-        <v>B171710</v>
+        <v>IR801997</v>
       </c>
       <c r="D4" t="str">
-        <v>NADIA BADRANE</v>
+        <v>NOUBAIL MOHAMMED</v>
       </c>
       <c r="E4" t="str">
         <v>non</v>
@@ -556,7 +556,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -565,21 +565,21 @@
         <v>--</v>
       </c>
       <c r="O4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>555/RRR/AV3</v>
+        <v>444/444</v>
       </c>
       <c r="B5" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C5" t="str">
-        <v>IB43905</v>
+        <v>B219321</v>
       </c>
       <c r="D5" t="str">
-        <v>NHILA BELGACEM</v>
+        <v>JEMAA HORMI</v>
       </c>
       <c r="E5" t="str">
         <v>non</v>
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -612,21 +612,21 @@
         <v>--</v>
       </c>
       <c r="O5">
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>555/RRR/AV3</v>
+        <v>444/444</v>
       </c>
       <c r="B6" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C6" t="str">
-        <v>B171710</v>
+        <v>IR801997</v>
       </c>
       <c r="D6" t="str">
-        <v>NADIA BADRANE</v>
+        <v>NOUBAIL MOHAMMED</v>
       </c>
       <c r="E6" t="str">
         <v>non</v>
@@ -638,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -655,25 +655,25 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" t="str">
-        <v>--</v>
+      <c r="N6">
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>555/RRR/AV3</v>
+        <v>444/444</v>
       </c>
       <c r="B7" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C7" t="str">
-        <v>IB43905</v>
+        <v>B219321</v>
       </c>
       <c r="D7" t="str">
-        <v>NHILA BELGACEM</v>
+        <v>JEMAA HORMI</v>
       </c>
       <c r="E7" t="str">
         <v>non</v>
@@ -685,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -702,16 +702,16 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7" t="str">
-        <v>--</v>
+      <c r="N7">
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>000/CCCC</v>
+        <v>000/CCCC/AV1</v>
       </c>
       <c r="B8" t="str">
         <v>Direction régionale</v>
@@ -731,20 +731,20 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>2000</v>
+      <c r="H8" t="str">
+        <v>--</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8">
-        <v>0</v>
+      <c r="J8" t="str">
+        <v>--</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>32000</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -753,59 +753,435 @@
         <v>--</v>
       </c>
       <c r="O8">
-        <v>2000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
+        <v>000/CCCC/AV1</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C9" t="str">
+        <v>BK646476</v>
+      </c>
+      <c r="D9" t="str">
+        <v>DOUNIA LAMKADDAM</v>
+      </c>
+      <c r="E9" t="str">
+        <v>non</v>
+      </c>
+      <c r="F9" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="str">
+        <v>--</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="str">
+        <v>--</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>4000</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" t="str">
+        <v>--</v>
+      </c>
+      <c r="O9">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>000/CCCC/AV1</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C10" t="str">
+        <v>BK646476</v>
+      </c>
+      <c r="D10" t="str">
+        <v>DOUNIA LAMKADDAM</v>
+      </c>
+      <c r="E10" t="str">
+        <v>non</v>
+      </c>
+      <c r="F10" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>2000</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="str">
+        <v>--</v>
+      </c>
+      <c r="O10">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>555/RRR/AV10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C11" t="str">
+        <v>B171710</v>
+      </c>
+      <c r="D11" t="str">
+        <v>NADIA BADRANE</v>
+      </c>
+      <c r="E11" t="str">
+        <v>non</v>
+      </c>
+      <c r="F11" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11" t="str">
+        <v>--</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="str">
+        <v>--</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>2000</v>
+      </c>
+      <c r="M11">
+        <v>200</v>
+      </c>
+      <c r="N11" t="str">
+        <v>--</v>
+      </c>
+      <c r="O11">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>555/RRR/AV10</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C12" t="str">
+        <v>IB43905</v>
+      </c>
+      <c r="D12" t="str">
+        <v>NHILA BELGACEM</v>
+      </c>
+      <c r="E12" t="str">
+        <v>non</v>
+      </c>
+      <c r="F12" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12" t="str">
+        <v>--</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="str">
+        <v>--</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>2000</v>
+      </c>
+      <c r="M12">
+        <v>200</v>
+      </c>
+      <c r="N12" t="str">
+        <v>--</v>
+      </c>
+      <c r="O12">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>555/RRR/AV10</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C13" t="str">
+        <v>B171710</v>
+      </c>
+      <c r="D13" t="str">
+        <v>NADIA BADRANE</v>
+      </c>
+      <c r="E13" t="str">
+        <v>non</v>
+      </c>
+      <c r="F13" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>8500</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>850</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" t="str">
+        <v>--</v>
+      </c>
+      <c r="O13">
+        <v>7650</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>555/RRR/AV10</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C14" t="str">
+        <v>IB43905</v>
+      </c>
+      <c r="D14" t="str">
+        <v>NHILA BELGACEM</v>
+      </c>
+      <c r="E14" t="str">
+        <v>non</v>
+      </c>
+      <c r="F14" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>8500</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>850</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14" t="str">
+        <v>--</v>
+      </c>
+      <c r="O14">
+        <v>7650</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>555/RRR/AV10</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C15" t="str">
+        <v>B171710</v>
+      </c>
+      <c r="D15" t="str">
+        <v>NADIA BADRANE</v>
+      </c>
+      <c r="E15" t="str">
+        <v>non</v>
+      </c>
+      <c r="F15" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15" t="str">
+        <v>--</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="str">
+        <v>--</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>2000</v>
+      </c>
+      <c r="M15">
+        <v>200</v>
+      </c>
+      <c r="N15" t="str">
+        <v>--</v>
+      </c>
+      <c r="O15">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>555/RRR/AV10</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C16" t="str">
+        <v>IB43905</v>
+      </c>
+      <c r="D16" t="str">
+        <v>NHILA BELGACEM</v>
+      </c>
+      <c r="E16" t="str">
+        <v>non</v>
+      </c>
+      <c r="F16" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16" t="str">
+        <v>--</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="str">
+        <v>--</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>2000</v>
+      </c>
+      <c r="M16">
+        <v>200</v>
+      </c>
+      <c r="N16" t="str">
+        <v>--</v>
+      </c>
+      <c r="O16">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B9" t="str">
+      <c r="B17" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C9" t="str">
+      <c r="C17" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D9" t="str">
+      <c r="D17" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E9" t="str">
+      <c r="E17" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F9" t="str">
+      <c r="F17" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G9" t="str">
+      <c r="G17" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H9">
-        <v>4000</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>36000</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>40000</v>
+      <c r="H17">
+        <v>22000</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1700</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>95000</v>
+      </c>
+      <c r="M17">
+        <v>800</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>114500</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>